<commit_message>
Beta version of DataParser
</commit_message>
<xml_diff>
--- a/main/Cases/Test1.xlsx
+++ b/main/Cases/Test1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.microsoftpersonalcontent.com/personal/119a6824fc18e16b/Documents/Documentos/projects/AGISTIN/T_04_06/agistin/main/Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/119a6824fc18e16b/Documentos/projects/AGISTIN/T_04_06/agistin/main/Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{B53D8EAC-DAFF-4D1F-984C-9B22EAF07FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CEB2E74-C02A-48CC-A499-B562C6528A8B}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{B53D8EAC-DAFF-4D1F-984C-9B22EAF07FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B1D7D9D-4F92-417E-A260-7D234896745B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Turb1</t>
   </si>
   <si>
-    <t>R1_OUT</t>
-  </si>
-  <si>
     <t>EB1</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>Qin,Reservoir1,Q;</t>
+  </si>
+  <si>
+    <t>R1out</t>
   </si>
 </sst>
 </file>
@@ -514,18 +514,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
         <v>100000000</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -551,18 +551,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>50000</v>
@@ -571,7 +571,7 @@
         <v>100000</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -647,7 +647,7 @@
         <v>480</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -670,7 +670,7 @@
         <v>510</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -705,7 +705,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -722,7 +722,7 @@
         <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -756,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +803,7 @@
         <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -832,7 +832,7 @@
         <v>0.9</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +861,7 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -872,7 +872,7 @@
         <v>0.9</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +901,7 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -912,7 +912,7 @@
         <v>0.85</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34E40F0-B7E1-4056-8BFB-2AABAC8389B5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,15 +938,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -958,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8D542D-EEC1-4E22-A5B2-39011ADAE04E}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -974,7 +974,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run() function and costs excel
</commit_message>
<xml_diff>
--- a/main/Cases/Test1.xlsx
+++ b/main/Cases/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/119a6824fc18e16b/Documentos/projects/AGISTIN/T_04_06/agistin/main/Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{B53D8EAC-DAFF-4D1F-984C-9B22EAF07FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B1D7D9D-4F92-417E-A260-7D234896745B}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{B53D8EAC-DAFF-4D1F-984C-9B22EAF07FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{414AB3C4-4878-43AC-8916-6A8A191E95EE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="10" xr2:uid="{A5667F64-109C-47C3-884E-1862F3FE77BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Source" sheetId="9" r:id="rId8"/>
     <sheet name="EB" sheetId="2" r:id="rId9"/>
     <sheet name="SolarPV" sheetId="10" r:id="rId10"/>
-    <sheet name="Switch" sheetId="11" r:id="rId11"/>
+    <sheet name="Battery" sheetId="12" r:id="rId11"/>
+    <sheet name="Switch" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -143,6 +144,21 @@
   </si>
   <si>
     <t>R1out</t>
+  </si>
+  <si>
+    <t>Battery1</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>Emax</t>
+  </si>
+  <si>
+    <t>SOCmin</t>
+  </si>
+  <si>
+    <t>SOCmax</t>
   </si>
 </sst>
 </file>
@@ -538,7 +554,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,6 +596,67 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89A51B1-8B3E-424C-A847-DA820C94EAD6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>7000</v>
+      </c>
+      <c r="C2">
+        <v>15000</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.98</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F4E95F-4697-4DBE-BA00-3D4090DC0192}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -924,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34E40F0-B7E1-4056-8BFB-2AABAC8389B5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>